<commit_message>
se realiza la transaccion de generar clave dinamica
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/clavedinamica/GestionarClaveDinamica.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/clavedinamica/GestionarClaveDinamica.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7695" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7695" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Inscribir" sheetId="1" r:id="rId1"/>
     <sheet name="Eliminar" sheetId="2" r:id="rId2"/>
+    <sheet name="Generar" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -114,6 +115,12 @@
   </si>
   <si>
     <t>User01</t>
+  </si>
+  <si>
+    <t>nombreUsuario</t>
+  </si>
+  <si>
+    <t>testing</t>
   </si>
 </sst>
 </file>
@@ -121,10 +128,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -149,21 +156,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -172,7 +179,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -186,8 +193,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -195,37 +263,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,55 +286,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -314,43 +321,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -362,139 +501,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -549,26 +556,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -612,26 +606,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -646,18 +620,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -667,131 +674,131 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1312,8 +1319,8 @@
   <sheetPr/>
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1"/>
@@ -1423,4 +1430,122 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1"/>
+    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="4" max="4" width="17.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:17">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1"/>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:17">
+      <c r="A2" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J2">
+      <formula1>Generar!$A$2:$A$3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>